<commit_message>
edit work in data
</commit_message>
<xml_diff>
--- a/ReportExcel/ReportExcel/bin/Debug/report.xlsx
+++ b/ReportExcel/ReportExcel/bin/Debug/report.xlsx
@@ -5,14 +5,14 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Отчет" sheetId="1" r:id="rId1"/>
+    <sheet name="Отчет" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Дата</t>
   </si>
@@ -24,6 +24,27 @@
   </si>
   <si>
     <t xml:space="preserve">Минимальное значение </t>
+  </si>
+  <si>
+    <t>20.08.2022 21:43:00</t>
+  </si>
+  <si>
+    <t>20.08.2022 21:44:00</t>
+  </si>
+  <si>
+    <t>20.08.2022 21:45:00</t>
+  </si>
+  <si>
+    <t>20.08.2022 21:46:00</t>
+  </si>
+  <si>
+    <t>20.08.2022 21:47:00</t>
+  </si>
+  <si>
+    <t>20.08.2022 23:06:00</t>
+  </si>
+  <si>
+    <t>20.08.2022 23:15:00</t>
   </si>
 </sst>
 </file>
@@ -273,20 +294,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:col>85</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="chart"/>
+        <xdr:cNvPr id="3" name="chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -326,13 +347,104 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0">
+        <v>9.759</v>
+      </c>
+      <c r="C2" s="0">
+        <v>5.325</v>
+      </c>
+      <c r="D2" s="0">
+        <v>0.786</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0">
+        <v>9.403</v>
+      </c>
+      <c r="C3" s="0">
+        <v>3.960888</v>
+      </c>
+      <c r="D3" s="0">
+        <v>0.357</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0">
+        <v>6.381</v>
+      </c>
+      <c r="C4" s="0">
+        <v>2.901444</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0.526</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0">
+        <v>8.899</v>
+      </c>
+      <c r="C5" s="0">
+        <v>4.654777</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.201</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0">
+        <v>9.607</v>
+      </c>
+      <c r="C6" s="0">
+        <v>6.057666</v>
+      </c>
+      <c r="D6" s="0">
+        <v>1.733</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0">
+        <v>7.506</v>
+      </c>
+      <c r="C7" s="0">
+        <v>4.092111</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1.466</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="0">
+        <v>9.555</v>
+      </c>
+      <c r="C8" s="0">
+        <v>6.769777</v>
+      </c>
+      <c r="D8" s="0">
+        <v>1.271</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
   <drawing r:id="rId1"/>

</xml_diff>